<commit_message>
Flap: add optional channel names for flap control signals
</commit_message>
<xml_diff>
--- a/modules/openfast-library/src/OutListParameters.xlsx
+++ b/modules/openfast-library/src/OutListParameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aplatt/software-development/GitHub/openfast-2/modules/openfast-library/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8201B900-4E0B-364E-BE9D-A2E4449D27BD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4F73B1-B116-584F-86CD-F8503A712EC6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="480" windowWidth="26580" windowHeight="23120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14540" yWindow="-22580" windowWidth="26580" windowHeight="22580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9477" uniqueCount="4813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9480" uniqueCount="4816">
   <si>
     <t>Category</t>
   </si>
@@ -14478,13 +14478,22 @@
   </si>
   <si>
     <t>ß</t>
+  </si>
+  <si>
+    <t>BlFlap1</t>
+  </si>
+  <si>
+    <t>BlFlap2</t>
+  </si>
+  <si>
+    <t>BlFlap3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -14504,6 +14513,12 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -34746,7 +34761,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -34795,7 +34810,9 @@
       <c r="B3" s="4" t="s">
         <v>4809</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>4813</v>
+      </c>
       <c r="D3" s="7" t="s">
         <v>4805</v>
       </c>
@@ -34810,7 +34827,9 @@
       <c r="B4" s="4" t="s">
         <v>4810</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>4814</v>
+      </c>
       <c r="D4" s="7" t="s">
         <v>4806</v>
       </c>
@@ -34825,7 +34844,9 @@
       <c r="B5" s="4" t="s">
         <v>4811</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>4815</v>
+      </c>
       <c r="D5" s="7" t="s">
         <v>4807</v>
       </c>
@@ -35142,6 +35163,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>